<commit_message>
Far east fed. dist. 15-16 (added)
15-16 data ready
</commit_message>
<xml_diff>
--- a/migforecasting/cities17-18/7/d1.xlsx
+++ b/migforecasting/cities17-18/7/d1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Albert\.spyder-py3\ITMO-2\migforecasting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Albert\.spyder-py3\ITMO-2\migforecasting\cities17-18\7\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -876,8 +876,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="I71" sqref="I71"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="H71" sqref="H71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1632,7 +1632,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <f>A48+1</f>
         <v>47</v>
@@ -1643,93 +1643,93 @@
       <c r="C49" s="5"/>
       <c r="D49" s="5"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <f t="shared" ref="A50:A86" si="0">A49+1</f>
         <v>48</v>
       </c>
-      <c r="B50" s="6">
+      <c r="C50" s="6">
         <v>222058.5</v>
       </c>
-      <c r="C50" s="6">
+      <c r="D50" s="6">
         <v>190741</v>
       </c>
-      <c r="D50" s="7">
+      <c r="E50" s="7">
         <v>186448.3</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
-      <c r="B51" s="6">
+      <c r="C51" s="6">
         <v>16337.4</v>
       </c>
-      <c r="C51" s="6">
+      <c r="D51" s="6">
         <v>10607.2</v>
       </c>
-      <c r="D51" s="7">
+      <c r="E51" s="7">
         <v>10060.6</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="B52" s="6">
+      <c r="C52" s="6">
         <v>50.6</v>
       </c>
-      <c r="C52" s="6">
+      <c r="D52" s="6">
         <v>44.6</v>
       </c>
-      <c r="D52" s="7">
+      <c r="E52" s="7">
         <v>46.1</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <f t="shared" si="0"/>
         <v>51</v>
       </c>
-      <c r="B53" s="6">
+      <c r="C53" s="6">
         <v>18.8</v>
       </c>
-      <c r="C53" s="6">
+      <c r="D53" s="6">
         <v>15.2</v>
       </c>
-      <c r="D53" s="7">
+      <c r="E53" s="7">
         <v>15.5</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
-      <c r="B54" s="5" t="s">
+      <c r="C54" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="C54" s="5"/>
       <c r="D54" s="5"/>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E54" s="5"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <f t="shared" si="0"/>
         <v>53</v>
       </c>
-      <c r="B55" s="6">
+      <c r="C55" s="6">
         <v>12991</v>
       </c>
-      <c r="C55" s="6">
+      <c r="D55" s="6">
         <v>12936</v>
       </c>
-      <c r="D55" s="7">
+      <c r="E55" s="7">
         <v>13094</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <f t="shared" si="0"/>
         <v>54</v>
@@ -1740,7 +1740,7 @@
       <c r="C56" s="5"/>
       <c r="D56" s="5"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <f t="shared" si="0"/>
         <v>55</v>
@@ -1749,67 +1749,67 @@
         <v>144</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <f t="shared" si="0"/>
         <v>56</v>
-      </c>
-      <c r="B58" s="6" t="s">
-        <v>141</v>
       </c>
       <c r="C58" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="D58" s="7" t="s">
+      <c r="D58" s="6" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E58" s="7" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <f t="shared" si="0"/>
         <v>57</v>
       </c>
-      <c r="B59" s="6">
+      <c r="C59" s="6">
         <v>43989.599999999999</v>
       </c>
-      <c r="C59" s="6">
+      <c r="D59" s="6">
         <v>48307.1</v>
       </c>
-      <c r="D59" s="7">
+      <c r="E59" s="7">
         <v>56096.2</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <f t="shared" si="0"/>
         <v>58</v>
       </c>
-      <c r="B60" s="6">
+      <c r="C60" s="6">
         <v>11416.9</v>
       </c>
-      <c r="C60" s="6">
+      <c r="D60" s="6">
         <v>11704.2</v>
       </c>
-      <c r="D60" s="7">
+      <c r="E60" s="7">
         <v>10471.299999999999</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <f t="shared" si="0"/>
         <v>59</v>
-      </c>
-      <c r="B61" s="6" t="s">
-        <v>141</v>
       </c>
       <c r="C61" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="D61" s="7" t="s">
+      <c r="D61" s="6" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E61" s="7" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <f t="shared" si="0"/>
         <v>60</v>
@@ -1818,121 +1818,121 @@
         <v>145</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <f t="shared" si="0"/>
         <v>61</v>
       </c>
-      <c r="B63" s="6">
+      <c r="C63" s="6">
         <v>2540.1</v>
       </c>
-      <c r="C63" s="6">
+      <c r="D63" s="6">
         <v>1197.2</v>
       </c>
-      <c r="D63" s="7">
+      <c r="E63" s="7">
         <v>1756.9</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <f t="shared" si="0"/>
         <v>62</v>
       </c>
-      <c r="B64" s="6">
+      <c r="C64" s="6">
         <v>119.6</v>
       </c>
-      <c r="C64" s="6">
+      <c r="D64" s="6">
         <v>147.30000000000001</v>
       </c>
-      <c r="D64" s="7">
+      <c r="E64" s="7">
         <v>147.5</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <f t="shared" si="0"/>
         <v>63</v>
       </c>
-      <c r="B65" s="6">
+      <c r="C65" s="6">
         <v>2241</v>
       </c>
-      <c r="C65" s="6">
+      <c r="D65" s="6">
         <v>2764</v>
       </c>
-      <c r="D65" s="7">
+      <c r="E65" s="7">
         <v>2080</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <f t="shared" si="0"/>
         <v>64</v>
       </c>
-      <c r="B66" s="6"/>
       <c r="C66" s="6"/>
-      <c r="D66" s="7"/>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D66" s="6"/>
+      <c r="E66" s="7"/>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <f t="shared" si="0"/>
         <v>65</v>
       </c>
-      <c r="B67" s="6">
+      <c r="C67" s="6">
         <v>82</v>
       </c>
-      <c r="C67" s="6">
+      <c r="D67" s="6">
         <v>120</v>
       </c>
-      <c r="D67" s="7" t="s">
+      <c r="E67" s="7" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <f t="shared" si="0"/>
         <v>66</v>
       </c>
-      <c r="B68" s="6">
+      <c r="C68" s="6">
         <v>100</v>
       </c>
-      <c r="C68" s="6" t="s">
+      <c r="D68" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="D68" s="7">
+      <c r="E68" s="7">
         <v>250</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <f t="shared" si="0"/>
         <v>67</v>
       </c>
-      <c r="B69" s="6">
+      <c r="C69" s="6">
         <v>10.1</v>
       </c>
-      <c r="C69" s="6">
+      <c r="D69" s="6">
         <v>12.6</v>
       </c>
-      <c r="D69" s="7">
+      <c r="E69" s="7">
         <v>20.2</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <f t="shared" si="0"/>
         <v>68</v>
       </c>
-      <c r="B70" s="6">
+      <c r="C70" s="6">
         <v>1.2</v>
       </c>
-      <c r="C70" s="6" t="s">
+      <c r="D70" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="D70" s="7">
+      <c r="E70" s="7">
         <v>0.5</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <f t="shared" si="0"/>
         <v>69</v>
@@ -1943,91 +1943,91 @@
       <c r="C71" s="5"/>
       <c r="D71" s="5"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <f t="shared" si="0"/>
         <v>70</v>
       </c>
-      <c r="B72" s="6">
+      <c r="C72" s="6">
         <v>17200.099999999999</v>
       </c>
-      <c r="C72" s="6">
+      <c r="D72" s="6">
         <v>18222.7</v>
       </c>
-      <c r="D72" s="7">
+      <c r="E72" s="7">
         <v>20053.2</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <f t="shared" si="0"/>
         <v>71</v>
       </c>
-      <c r="B73" s="6">
+      <c r="C73" s="6">
         <v>109.3</v>
       </c>
-      <c r="C73" s="6">
+      <c r="D73" s="6">
         <v>102.4</v>
       </c>
-      <c r="D73" s="7">
+      <c r="E73" s="7">
         <v>104.2</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <f t="shared" si="0"/>
         <v>72</v>
       </c>
-      <c r="B74" s="6">
+      <c r="C74" s="6">
         <v>905.2</v>
       </c>
-      <c r="C74" s="6">
+      <c r="D74" s="6">
         <v>478.6</v>
       </c>
-      <c r="D74" s="7">
+      <c r="E74" s="7">
         <v>525.9</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <f t="shared" si="0"/>
         <v>73</v>
       </c>
-      <c r="B75" s="3">
+      <c r="C75" s="3">
         <v>110.4</v>
       </c>
-      <c r="C75" s="3">
+      <c r="D75" s="3">
         <v>54.6</v>
       </c>
-      <c r="D75" s="4">
+      <c r="E75" s="4">
         <v>104</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <f t="shared" si="0"/>
         <v>74</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <f t="shared" si="0"/>
         <v>75</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <f t="shared" si="0"/>
         <v>76</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <f t="shared" si="0"/>
         <v>77</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <f t="shared" si="0"/>
         <v>78</v>

</xml_diff>